<commit_message>
he actualizado las correspondencias del SIOSE
</commit_message>
<xml_diff>
--- a/Correspondencias_SIOSE - modificada (v2).xlsx
+++ b/Correspondencias_SIOSE - modificada (v2).xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5836" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5918" uniqueCount="1039">
   <si>
     <t>COD_JER</t>
   </si>
@@ -3143,12 +3143,81 @@
   <si>
     <t>RIOS Y CAUCES - LAMINA DE AGUA</t>
   </si>
+  <si>
+    <t>REVISAR</t>
+  </si>
+  <si>
+    <t>DEFINITIVA</t>
+  </si>
+  <si>
+    <t>Tejido urbano</t>
+  </si>
+  <si>
+    <t>Zonas industriales y comerciales</t>
+  </si>
+  <si>
+    <t>Infraestructuras de comunicaciones</t>
+  </si>
+  <si>
+    <t>Otras infraestructuras tecnicas</t>
+  </si>
+  <si>
+    <t>Zonas verdes y espacios de ocio</t>
+  </si>
+  <si>
+    <t>Marisma con vegetacion</t>
+  </si>
+  <si>
+    <t>Marisma sin vegetacion</t>
+  </si>
+  <si>
+    <t>Rios y cauces</t>
+  </si>
+  <si>
+    <t>Cultivos en invernadero</t>
+  </si>
+  <si>
+    <t>Formacion arbolada</t>
+  </si>
+  <si>
+    <t>Playas, dunas y arenales</t>
+  </si>
+  <si>
+    <t>Secano</t>
+  </si>
+  <si>
+    <t>Regadio</t>
+  </si>
+  <si>
+    <t>Areas con fuertes procesos erosivos</t>
+  </si>
+  <si>
+    <t>Zonas sin vegetacion por roturacion</t>
+  </si>
+  <si>
+    <t>Sin asignacion</t>
+  </si>
+  <si>
+    <t>Cultivo herbaceo distinto de arroz</t>
+  </si>
+  <si>
+    <t>Agricola residencial</t>
+  </si>
+  <si>
+    <t>Agricola/ganadero</t>
+  </si>
+  <si>
+    <t>Zona de extraccion o vertido</t>
+  </si>
+  <si>
+    <t>Lamina de agua artificial</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3271,6 +3340,12 @@
       <name val="Open Sans"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -3471,7 +3546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3559,6 +3634,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3812,16 +3890,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>25</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>54428</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>38</xdr:col>
+      <xdr:col>40</xdr:col>
       <xdr:colOff>378219</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>7588</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>184481</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -23141,7 +23219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E193"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
@@ -24880,10 +24958,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38:D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -24891,27 +24969,28 @@
     <col min="1" max="1" width="69" customWidth="1"/>
     <col min="2" max="2" width="6.25" customWidth="1"/>
     <col min="3" max="3" width="44.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.375" style="42" customWidth="1"/>
-    <col min="5" max="5" width="64.25" style="13" customWidth="1"/>
-    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44.25" customWidth="1"/>
+    <col min="4" max="5" width="44.25" customWidth="1"/>
+    <col min="6" max="6" width="33.375" style="42" customWidth="1"/>
+    <col min="7" max="7" width="64.25" style="13" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.25" customWidth="1"/>
+    <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17" customWidth="1"/>
-    <col min="18" max="18" width="4.75" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.25" customWidth="1"/>
-    <col min="20" max="20" width="2.875" customWidth="1"/>
-    <col min="21" max="21" width="4.25" customWidth="1"/>
+    <col min="17" max="17" width="33.375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17" customWidth="1"/>
+    <col min="20" max="20" width="4.75" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.25" customWidth="1"/>
+    <col min="22" max="22" width="2.875" customWidth="1"/>
+    <col min="23" max="23" width="4.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:7" ht="15">
       <c r="A1" s="25" t="s">
         <v>977</v>
       </c>
@@ -24921,14 +25000,17 @@
       <c r="C1" s="16" t="s">
         <v>986</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>987</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="G1" s="45" t="s">
         <v>994</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15">
+    <row r="2" spans="1:7" ht="15">
       <c r="A2" s="4" t="s">
         <v>753</v>
       </c>
@@ -24938,9 +25020,16 @@
       <c r="C2" s="10" t="s">
         <v>931</v>
       </c>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="3" spans="1:5" ht="15">
+      <c r="D2" s="57" t="s">
+        <v>1018</v>
+      </c>
+      <c r="E2" t="str">
+        <f>LOWER(D2)</f>
+        <v>tejido urbano</v>
+      </c>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" s="4" t="s">
         <v>753</v>
       </c>
@@ -24950,9 +25039,12 @@
       <c r="C3" s="10" t="s">
         <v>928</v>
       </c>
-      <c r="D3" s="13"/>
-    </row>
-    <row r="4" spans="1:5" ht="15">
+      <c r="D3" s="57" t="s">
+        <v>1018</v>
+      </c>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="1:7" ht="15">
       <c r="A4" s="4" t="s">
         <v>753</v>
       </c>
@@ -24962,8 +25054,11 @@
       <c r="C4" s="10" t="s">
         <v>969</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15">
+      <c r="D4" s="57" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15">
       <c r="A5" s="4" t="s">
         <v>753</v>
       </c>
@@ -24973,8 +25068,11 @@
       <c r="C5" s="10" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15">
+      <c r="D5" s="57" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15">
       <c r="A6" s="4" t="s">
         <v>753</v>
       </c>
@@ -24984,8 +25082,11 @@
       <c r="C6" s="10" t="s">
         <v>933</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15">
+      <c r="D6" s="57" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15">
       <c r="A7" s="4" t="s">
         <v>753</v>
       </c>
@@ -24995,8 +25096,11 @@
       <c r="C7" s="10" t="s">
         <v>898</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="D7" s="57" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15">
       <c r="A8" s="1" t="s">
         <v>1010</v>
       </c>
@@ -25006,8 +25110,11 @@
       <c r="C8" s="23" t="s">
         <v>934</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15">
+      <c r="D8" s="57" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15">
       <c r="A9" s="1" t="s">
         <v>756</v>
       </c>
@@ -25017,8 +25124,11 @@
       <c r="C9" s="20" t="s">
         <v>925</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15">
+      <c r="D9" s="57" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15">
       <c r="A10" s="4" t="s">
         <v>757</v>
       </c>
@@ -25028,8 +25138,11 @@
       <c r="C10" s="10" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15">
+      <c r="D10" s="57" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15">
       <c r="A11" s="4" t="s">
         <v>757</v>
       </c>
@@ -25039,8 +25152,11 @@
       <c r="C11" s="10" t="s">
         <v>938</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15">
+      <c r="D11" s="57" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15">
       <c r="A12" s="4" t="s">
         <v>757</v>
       </c>
@@ -25050,8 +25166,11 @@
       <c r="C12" s="10" t="s">
         <v>955</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D12" s="57" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A13" s="4" t="s">
         <v>757</v>
       </c>
@@ -25061,9 +25180,13 @@
       <c r="C13" s="10" t="s">
         <v>912</v>
       </c>
-      <c r="D13" s="42"/>
-    </row>
-    <row r="14" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D13" s="57" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E13"/>
+      <c r="F13" s="42"/>
+    </row>
+    <row r="14" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A14" s="4" t="s">
         <v>757</v>
       </c>
@@ -25073,9 +25196,13 @@
       <c r="C14" s="10" t="s">
         <v>899</v>
       </c>
-      <c r="D14" s="42"/>
-    </row>
-    <row r="15" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D14" s="57" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E14"/>
+      <c r="F14" s="42"/>
+    </row>
+    <row r="15" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A15" s="4" t="s">
         <v>758</v>
       </c>
@@ -25085,9 +25212,13 @@
       <c r="C15" s="23" t="s">
         <v>927</v>
       </c>
-      <c r="D15" s="42"/>
-    </row>
-    <row r="16" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D15" s="57" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E15"/>
+      <c r="F15" s="42"/>
+    </row>
+    <row r="16" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A16" s="4" t="s">
         <v>758</v>
       </c>
@@ -25097,9 +25228,13 @@
       <c r="C16" s="23" t="s">
         <v>892</v>
       </c>
-      <c r="D16" s="42"/>
-    </row>
-    <row r="17" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D16" s="57" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E16"/>
+      <c r="F16" s="42"/>
+    </row>
+    <row r="17" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A17" s="4" t="s">
         <v>758</v>
       </c>
@@ -25109,8 +25244,12 @@
       <c r="C17" s="23" t="s">
         <v>891</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D17" s="57" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E17"/>
+    </row>
+    <row r="18" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A18" s="1" t="s">
         <v>763</v>
       </c>
@@ -25120,9 +25259,13 @@
       <c r="C18" s="20" t="s">
         <v>940</v>
       </c>
-      <c r="D18" s="42"/>
-    </row>
-    <row r="19" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D18" s="57" t="s">
+        <v>940</v>
+      </c>
+      <c r="E18"/>
+      <c r="F18" s="42"/>
+    </row>
+    <row r="19" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A19" s="4" t="s">
         <v>763</v>
       </c>
@@ -25132,9 +25275,13 @@
       <c r="C19" s="10" t="s">
         <v>958</v>
       </c>
-      <c r="D19" s="42"/>
-    </row>
-    <row r="20" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D19" s="57" t="s">
+        <v>1021</v>
+      </c>
+      <c r="E19"/>
+      <c r="F19" s="42"/>
+    </row>
+    <row r="20" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A20" s="4" t="s">
         <v>763</v>
       </c>
@@ -25144,8 +25291,12 @@
       <c r="C20" s="10" t="s">
         <v>953</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D20" s="57" t="s">
+        <v>1021</v>
+      </c>
+      <c r="E20"/>
+    </row>
+    <row r="21" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A21" s="4" t="s">
         <v>763</v>
       </c>
@@ -25155,9 +25306,13 @@
       <c r="C21" s="10" t="s">
         <v>935</v>
       </c>
-      <c r="D21" s="42"/>
-    </row>
-    <row r="22" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D21" s="57" t="s">
+        <v>1021</v>
+      </c>
+      <c r="E21"/>
+      <c r="F21" s="42"/>
+    </row>
+    <row r="22" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A22" s="1" t="s">
         <v>763</v>
       </c>
@@ -25167,9 +25322,13 @@
       <c r="C22" s="20" t="s">
         <v>907</v>
       </c>
-      <c r="D22" s="42"/>
-    </row>
-    <row r="23" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D22" s="57" t="s">
+        <v>1036</v>
+      </c>
+      <c r="E22"/>
+      <c r="F22" s="42"/>
+    </row>
+    <row r="23" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A23" s="1" t="s">
         <v>764</v>
       </c>
@@ -25179,9 +25338,13 @@
       <c r="C23" s="20" t="s">
         <v>959</v>
       </c>
-      <c r="D23" s="42"/>
-    </row>
-    <row r="24" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D23" s="57" t="s">
+        <v>959</v>
+      </c>
+      <c r="E23"/>
+      <c r="F23" s="42"/>
+    </row>
+    <row r="24" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A24" s="1" t="s">
         <v>764</v>
       </c>
@@ -25191,9 +25354,13 @@
       <c r="C24" s="20" t="s">
         <v>937</v>
       </c>
-      <c r="E24" s="13"/>
-    </row>
-    <row r="25" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D24" s="57" t="s">
+        <v>1037</v>
+      </c>
+      <c r="E24"/>
+      <c r="G24" s="13"/>
+    </row>
+    <row r="25" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A25" s="1" t="s">
         <v>765</v>
       </c>
@@ -25203,9 +25370,13 @@
       <c r="C25" s="20" t="s">
         <v>946</v>
       </c>
-      <c r="E25" s="13"/>
-    </row>
-    <row r="26" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D25" s="57" t="s">
+        <v>946</v>
+      </c>
+      <c r="E25"/>
+      <c r="G25" s="13"/>
+    </row>
+    <row r="26" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A26" s="4" t="s">
         <v>135</v>
       </c>
@@ -25215,9 +25386,13 @@
       <c r="C26" s="23" t="s">
         <v>929</v>
       </c>
-      <c r="E26" s="13"/>
-    </row>
-    <row r="27" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D26" s="57" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E26"/>
+      <c r="G26" s="13"/>
+    </row>
+    <row r="27" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A27" s="4" t="s">
         <v>135</v>
       </c>
@@ -25227,9 +25402,13 @@
       <c r="C27" s="23" t="s">
         <v>910</v>
       </c>
-      <c r="E27" s="13"/>
-    </row>
-    <row r="28" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D27" s="57" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E27"/>
+      <c r="G27" s="13"/>
+    </row>
+    <row r="28" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A28" s="4" t="s">
         <v>135</v>
       </c>
@@ -25239,9 +25418,13 @@
       <c r="C28" s="23" t="s">
         <v>924</v>
       </c>
-      <c r="E28" s="13"/>
-    </row>
-    <row r="29" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D28" s="57" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E28"/>
+      <c r="G28" s="13"/>
+    </row>
+    <row r="29" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A29" s="4" t="s">
         <v>135</v>
       </c>
@@ -25251,9 +25434,13 @@
       <c r="C29" s="23" t="s">
         <v>951</v>
       </c>
-      <c r="E29" s="13"/>
-    </row>
-    <row r="30" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D29" s="57" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E29"/>
+      <c r="G29" s="13"/>
+    </row>
+    <row r="30" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A30" s="4" t="s">
         <v>135</v>
       </c>
@@ -25263,9 +25450,13 @@
       <c r="C30" s="23" t="s">
         <v>957</v>
       </c>
-      <c r="E30" s="13"/>
-    </row>
-    <row r="31" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D30" s="57" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E30"/>
+      <c r="G30" s="13"/>
+    </row>
+    <row r="31" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A31" s="4" t="s">
         <v>135</v>
       </c>
@@ -25275,9 +25466,13 @@
       <c r="C31" s="23" t="s">
         <v>966</v>
       </c>
-      <c r="E31" s="13"/>
-    </row>
-    <row r="32" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D31" s="57" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E31"/>
+      <c r="G31" s="13"/>
+    </row>
+    <row r="32" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A32" s="4" t="s">
         <v>135</v>
       </c>
@@ -25287,9 +25482,13 @@
       <c r="C32" s="23" t="s">
         <v>967</v>
       </c>
-      <c r="E32" s="13"/>
-    </row>
-    <row r="33" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D32" s="57" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E32"/>
+      <c r="G32" s="13"/>
+    </row>
+    <row r="33" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A33" s="4" t="s">
         <v>135</v>
       </c>
@@ -25299,9 +25498,13 @@
       <c r="C33" s="23" t="s">
         <v>968</v>
       </c>
-      <c r="E33" s="13"/>
-    </row>
-    <row r="34" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D33" s="57" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E33"/>
+      <c r="G33" s="13"/>
+    </row>
+    <row r="34" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A34" s="4" t="s">
         <v>1011</v>
       </c>
@@ -25311,9 +25514,13 @@
       <c r="C34" s="10" t="s">
         <v>944</v>
       </c>
-      <c r="E34" s="13"/>
-    </row>
-    <row r="35" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D34" s="57" t="s">
+        <v>1023</v>
+      </c>
+      <c r="E34"/>
+      <c r="G34" s="13"/>
+    </row>
+    <row r="35" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A35" s="4" t="s">
         <v>1011</v>
       </c>
@@ -25323,9 +25530,13 @@
       <c r="C35" s="23" t="s">
         <v>965</v>
       </c>
-      <c r="E35" s="13"/>
-    </row>
-    <row r="36" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D35" s="57" t="s">
+        <v>1023</v>
+      </c>
+      <c r="E35"/>
+      <c r="G35" s="13"/>
+    </row>
+    <row r="36" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A36" s="4" t="s">
         <v>1012</v>
       </c>
@@ -25335,9 +25546,13 @@
       <c r="C36" s="10" t="s">
         <v>964</v>
       </c>
-      <c r="E36" s="13"/>
-    </row>
-    <row r="37" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D36" s="57" t="s">
+        <v>1024</v>
+      </c>
+      <c r="E36"/>
+      <c r="G36" s="13"/>
+    </row>
+    <row r="37" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A37" s="4" t="s">
         <v>1012</v>
       </c>
@@ -25347,9 +25562,13 @@
       <c r="C37" s="10" t="s">
         <v>970</v>
       </c>
-      <c r="E37" s="13"/>
-    </row>
-    <row r="38" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D37" s="57" t="s">
+        <v>1024</v>
+      </c>
+      <c r="E37"/>
+      <c r="G37" s="13"/>
+    </row>
+    <row r="38" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A38" s="56" t="s">
         <v>1013</v>
       </c>
@@ -25359,9 +25578,13 @@
       <c r="C38" s="31" t="s">
         <v>950</v>
       </c>
-      <c r="E38" s="13"/>
-    </row>
-    <row r="39" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D38" s="57" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E38"/>
+      <c r="G38" s="13"/>
+    </row>
+    <row r="39" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A39" s="56" t="s">
         <v>1013</v>
       </c>
@@ -25371,9 +25594,13 @@
       <c r="C39" s="31" t="s">
         <v>952</v>
       </c>
-      <c r="E39" s="13"/>
-    </row>
-    <row r="40" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D39" s="57" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E39"/>
+      <c r="G39" s="13"/>
+    </row>
+    <row r="40" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A40" s="41" t="s">
         <v>780</v>
       </c>
@@ -25383,9 +25610,13 @@
       <c r="C40" s="20" t="s">
         <v>947</v>
       </c>
-      <c r="E40" s="13"/>
-    </row>
-    <row r="41" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D40" s="57" t="s">
+        <v>947</v>
+      </c>
+      <c r="E40"/>
+      <c r="G40" s="13"/>
+    </row>
+    <row r="41" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A41" s="1" t="s">
         <v>781</v>
       </c>
@@ -25395,9 +25626,13 @@
       <c r="C41" s="20" t="s">
         <v>916</v>
       </c>
-      <c r="E41" s="13"/>
-    </row>
-    <row r="42" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D41" s="57" t="s">
+        <v>916</v>
+      </c>
+      <c r="E41"/>
+      <c r="G41" s="13"/>
+    </row>
+    <row r="42" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A42" s="4" t="s">
         <v>1015</v>
       </c>
@@ -25407,9 +25642,13 @@
       <c r="C42" s="10" t="s">
         <v>961</v>
       </c>
-      <c r="E42" s="13"/>
-    </row>
-    <row r="43" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D42" s="57" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E42"/>
+      <c r="G42" s="13"/>
+    </row>
+    <row r="43" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A43" s="4" t="s">
         <v>1015</v>
       </c>
@@ -25419,9 +25658,13 @@
       <c r="C43" s="10" t="s">
         <v>960</v>
       </c>
-      <c r="E43" s="13"/>
-    </row>
-    <row r="44" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D43" s="57" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E43"/>
+      <c r="G43" s="13"/>
+    </row>
+    <row r="44" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A44" s="41" t="s">
         <v>1014</v>
       </c>
@@ -25431,9 +25674,13 @@
       <c r="C44" s="20" t="s">
         <v>897</v>
       </c>
-      <c r="E44" s="13"/>
-    </row>
-    <row r="45" spans="1:5" s="13" customFormat="1">
+      <c r="D44" s="57" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E44"/>
+      <c r="G44" s="13"/>
+    </row>
+    <row r="45" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A45" s="41" t="s">
         <v>1014</v>
       </c>
@@ -25443,9 +25690,13 @@
       <c r="C45" s="23" t="s">
         <v>973</v>
       </c>
-      <c r="D45" s="42"/>
-    </row>
-    <row r="46" spans="1:5" s="13" customFormat="1">
+      <c r="D45" s="57" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E45"/>
+      <c r="F45" s="42"/>
+    </row>
+    <row r="46" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A46" s="41" t="s">
         <v>1014</v>
       </c>
@@ -25455,9 +25706,13 @@
       <c r="C46" s="23" t="s">
         <v>911</v>
       </c>
-      <c r="D46" s="42"/>
-    </row>
-    <row r="47" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D46" s="57" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E46"/>
+      <c r="F46" s="42"/>
+    </row>
+    <row r="47" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A47" s="41" t="s">
         <v>786</v>
       </c>
@@ -25467,9 +25722,13 @@
       <c r="C47" s="20" t="s">
         <v>956</v>
       </c>
-      <c r="D47" s="42"/>
-    </row>
-    <row r="48" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D47" s="57" t="s">
+        <v>956</v>
+      </c>
+      <c r="E47"/>
+      <c r="F47" s="42"/>
+    </row>
+    <row r="48" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A48" s="41" t="s">
         <v>786</v>
       </c>
@@ -25479,9 +25738,13 @@
       <c r="C48" s="20" t="s">
         <v>906</v>
       </c>
-      <c r="D48" s="42"/>
-    </row>
-    <row r="49" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D48" s="57" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E48"/>
+      <c r="F48" s="42"/>
+    </row>
+    <row r="49" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A49" s="41" t="s">
         <v>787</v>
       </c>
@@ -25491,9 +25754,13 @@
       <c r="C49" s="20" t="s">
         <v>902</v>
       </c>
-      <c r="D49" s="42"/>
-    </row>
-    <row r="50" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D49" s="57" t="s">
+        <v>902</v>
+      </c>
+      <c r="E49"/>
+      <c r="F49" s="42"/>
+    </row>
+    <row r="50" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A50" s="1" t="s">
         <v>789</v>
       </c>
@@ -25503,9 +25770,13 @@
       <c r="C50" s="20" t="s">
         <v>941</v>
       </c>
-      <c r="D50" s="42"/>
-    </row>
-    <row r="51" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D50" s="57" t="s">
+        <v>941</v>
+      </c>
+      <c r="E50"/>
+      <c r="F50" s="42"/>
+    </row>
+    <row r="51" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A51" s="1" t="s">
         <v>790</v>
       </c>
@@ -25515,9 +25786,13 @@
       <c r="C51" s="20" t="s">
         <v>914</v>
       </c>
-      <c r="D51" s="42"/>
-    </row>
-    <row r="52" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D51" s="57" t="s">
+        <v>914</v>
+      </c>
+      <c r="E51"/>
+      <c r="F51" s="42"/>
+    </row>
+    <row r="52" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A52" s="1" t="s">
         <v>283</v>
       </c>
@@ -25527,11 +25802,15 @@
       <c r="C52" s="27" t="s">
         <v>918</v>
       </c>
-      <c r="D52" s="43" t="s">
+      <c r="D52" s="57" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E52"/>
+      <c r="F52" s="43" t="s">
         <v>982</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="13" customFormat="1" ht="15">
+    <row r="53" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A53" s="4" t="s">
         <v>981</v>
       </c>
@@ -25541,9 +25820,13 @@
       <c r="C53" s="10" t="s">
         <v>939</v>
       </c>
-      <c r="D53" s="42"/>
-    </row>
-    <row r="54" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D53" s="57" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E53"/>
+      <c r="F53" s="42"/>
+    </row>
+    <row r="54" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A54" s="4" t="s">
         <v>796</v>
       </c>
@@ -25553,9 +25836,13 @@
       <c r="C54" s="19" t="s">
         <v>923</v>
       </c>
-      <c r="D54" s="42"/>
-    </row>
-    <row r="55" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D54" s="57" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E54"/>
+      <c r="F54" s="42"/>
+    </row>
+    <row r="55" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A55" s="4" t="s">
         <v>801</v>
       </c>
@@ -25565,11 +25852,13 @@
       <c r="C55" s="10" t="s">
         <v>893</v>
       </c>
-      <c r="D55" s="43" t="s">
-        <v>984</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D55" s="57" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E55"/>
+      <c r="F55" s="43"/>
+    </row>
+    <row r="56" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A56" s="4" t="s">
         <v>801</v>
       </c>
@@ -25579,9 +25868,13 @@
       <c r="C56" s="10" t="s">
         <v>900</v>
       </c>
-      <c r="D56" s="44"/>
-    </row>
-    <row r="57" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D56" s="57" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E56"/>
+      <c r="F56" s="44"/>
+    </row>
+    <row r="57" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A57" s="4" t="s">
         <v>985</v>
       </c>
@@ -25591,11 +25884,13 @@
       <c r="C57" s="10" t="s">
         <v>971</v>
       </c>
-      <c r="D57" s="43" t="s">
-        <v>983</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D57" s="57" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E57"/>
+      <c r="F57" s="43"/>
+    </row>
+    <row r="58" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A58" s="1" t="s">
         <v>810</v>
       </c>
@@ -25605,9 +25900,13 @@
       <c r="C58" s="20" t="s">
         <v>909</v>
       </c>
-      <c r="D58" s="42"/>
-    </row>
-    <row r="59" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D58" s="57" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E58"/>
+      <c r="F58" s="42"/>
+    </row>
+    <row r="59" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A59" s="1" t="s">
         <v>811</v>
       </c>
@@ -25617,9 +25916,13 @@
       <c r="C59" s="20" t="s">
         <v>904</v>
       </c>
-      <c r="D59" s="42"/>
-    </row>
-    <row r="60" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D59" s="57" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E59"/>
+      <c r="F59" s="42"/>
+    </row>
+    <row r="60" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A60" s="1" t="s">
         <v>835</v>
       </c>
@@ -25629,9 +25932,13 @@
       <c r="C60" s="20" t="s">
         <v>921</v>
       </c>
-      <c r="E60" s="13"/>
-    </row>
-    <row r="61" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D60" s="57" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E60"/>
+      <c r="G60" s="13"/>
+    </row>
+    <row r="61" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A61" s="1" t="s">
         <v>836</v>
       </c>
@@ -25641,9 +25948,13 @@
       <c r="C61" s="20" t="s">
         <v>926</v>
       </c>
-      <c r="E61" s="13"/>
-    </row>
-    <row r="62" spans="1:5" s="42" customFormat="1">
+      <c r="D61" s="57" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E61"/>
+      <c r="G61" s="13"/>
+    </row>
+    <row r="62" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A62" s="25" t="s">
         <v>846</v>
       </c>
@@ -25653,9 +25964,13 @@
       <c r="C62" s="23" t="s">
         <v>949</v>
       </c>
-      <c r="E62" s="13"/>
-    </row>
-    <row r="63" spans="1:5" s="42" customFormat="1">
+      <c r="D62" s="57" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E62"/>
+      <c r="G62" s="13"/>
+    </row>
+    <row r="63" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A63" s="25" t="s">
         <v>847</v>
       </c>
@@ -25665,9 +25980,13 @@
       <c r="C63" s="23" t="s">
         <v>948</v>
       </c>
-      <c r="E63" s="13"/>
-    </row>
-    <row r="64" spans="1:5" s="42" customFormat="1">
+      <c r="D63" s="57" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E63"/>
+      <c r="G63" s="13"/>
+    </row>
+    <row r="64" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A64" s="25" t="s">
         <v>858</v>
       </c>
@@ -25677,9 +25996,13 @@
       <c r="C64" s="23" t="s">
         <v>943</v>
       </c>
-      <c r="E64" s="13"/>
-    </row>
-    <row r="65" spans="1:5" s="42" customFormat="1">
+      <c r="D64" s="57" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E64"/>
+      <c r="G64" s="13"/>
+    </row>
+    <row r="65" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A65" s="25" t="s">
         <v>859</v>
       </c>
@@ -25689,9 +26012,13 @@
       <c r="C65" s="23" t="s">
         <v>920</v>
       </c>
-      <c r="E65" s="13"/>
-    </row>
-    <row r="66" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D65" s="57" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E65"/>
+      <c r="G65" s="13"/>
+    </row>
+    <row r="66" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A66" s="25" t="s">
         <v>860</v>
       </c>
@@ -25701,9 +26028,13 @@
       <c r="C66" s="20" t="s">
         <v>936</v>
       </c>
-      <c r="E66" s="13"/>
-    </row>
-    <row r="67" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D66" s="57" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E66"/>
+      <c r="G66" s="13"/>
+    </row>
+    <row r="67" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A67" s="25" t="s">
         <v>861</v>
       </c>
@@ -25713,9 +26044,13 @@
       <c r="C67" s="20" t="s">
         <v>932</v>
       </c>
-      <c r="E67" s="13"/>
-    </row>
-    <row r="68" spans="1:5" s="42" customFormat="1">
+      <c r="D67" s="57" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E67"/>
+      <c r="G67" s="13"/>
+    </row>
+    <row r="68" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A68" s="1" t="s">
         <v>870</v>
       </c>
@@ -25725,9 +26060,13 @@
       <c r="C68" s="23" t="s">
         <v>919</v>
       </c>
-      <c r="E68" s="13"/>
-    </row>
-    <row r="69" spans="1:5" s="42" customFormat="1">
+      <c r="D68" s="57" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E68"/>
+      <c r="G68" s="13"/>
+    </row>
+    <row r="69" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A69" s="1" t="s">
         <v>871</v>
       </c>
@@ -25737,9 +26076,13 @@
       <c r="C69" s="23" t="s">
         <v>942</v>
       </c>
-      <c r="E69" s="13"/>
-    </row>
-    <row r="70" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D69" s="57" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E69"/>
+      <c r="G69" s="13"/>
+    </row>
+    <row r="70" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A70" s="1" t="s">
         <v>872</v>
       </c>
@@ -25749,9 +26092,13 @@
       <c r="C70" s="20" t="s">
         <v>962</v>
       </c>
-      <c r="E70" s="13"/>
-    </row>
-    <row r="71" spans="1:5" s="42" customFormat="1" ht="15">
+      <c r="D70" s="57" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E70"/>
+      <c r="G70" s="13"/>
+    </row>
+    <row r="71" spans="1:7" s="42" customFormat="1" ht="15">
       <c r="A71" s="1" t="s">
         <v>873</v>
       </c>
@@ -25761,9 +26108,13 @@
       <c r="C71" s="20" t="s">
         <v>945</v>
       </c>
-      <c r="E71" s="13"/>
-    </row>
-    <row r="72" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D71" s="57" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E71"/>
+      <c r="G71" s="13"/>
+    </row>
+    <row r="72" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A72" s="1" t="s">
         <v>880</v>
       </c>
@@ -25773,9 +26124,13 @@
       <c r="C72" s="20" t="s">
         <v>913</v>
       </c>
-      <c r="D72" s="42"/>
-    </row>
-    <row r="73" spans="1:5" s="13" customFormat="1">
+      <c r="D72" s="57" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E72"/>
+      <c r="F72" s="42"/>
+    </row>
+    <row r="73" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A73" s="1" t="s">
         <v>882</v>
       </c>
@@ -25785,9 +26140,13 @@
       <c r="C73" s="23" t="s">
         <v>901</v>
       </c>
-      <c r="D73" s="42"/>
-    </row>
-    <row r="74" spans="1:5" s="13" customFormat="1">
+      <c r="D73" s="57" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E73"/>
+      <c r="F73" s="42"/>
+    </row>
+    <row r="74" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A74" s="1" t="s">
         <v>883</v>
       </c>
@@ -25797,9 +26156,13 @@
       <c r="C74" s="23" t="s">
         <v>915</v>
       </c>
-      <c r="D74" s="42"/>
-    </row>
-    <row r="75" spans="1:5" s="13" customFormat="1">
+      <c r="D74" s="57" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E74"/>
+      <c r="F74" s="42"/>
+    </row>
+    <row r="75" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A75" s="1" t="s">
         <v>884</v>
       </c>
@@ -25809,9 +26172,13 @@
       <c r="C75" s="23" t="s">
         <v>908</v>
       </c>
-      <c r="D75" s="42"/>
-    </row>
-    <row r="76" spans="1:5" s="13" customFormat="1">
+      <c r="D75" s="57" t="s">
+        <v>1006</v>
+      </c>
+      <c r="E75"/>
+      <c r="F75" s="42"/>
+    </row>
+    <row r="76" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A76" s="1" t="s">
         <v>885</v>
       </c>
@@ -25821,9 +26188,13 @@
       <c r="C76" s="23" t="s">
         <v>896</v>
       </c>
-      <c r="D76" s="42"/>
-    </row>
-    <row r="77" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D76" s="57" t="s">
+        <v>1006</v>
+      </c>
+      <c r="E76"/>
+      <c r="F76" s="42"/>
+    </row>
+    <row r="77" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A77" s="4" t="s">
         <v>886</v>
       </c>
@@ -25833,8 +26204,12 @@
       <c r="C77" s="10" t="s">
         <v>894</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D77" s="57" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E77"/>
+    </row>
+    <row r="78" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A78" s="4" t="s">
         <v>886</v>
       </c>
@@ -25844,9 +26219,13 @@
       <c r="C78" s="10" t="s">
         <v>895</v>
       </c>
-      <c r="D78" s="42"/>
-    </row>
-    <row r="79" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D78" s="57" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E78"/>
+      <c r="F78" s="42"/>
+    </row>
+    <row r="79" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A79" s="4" t="s">
         <v>886</v>
       </c>
@@ -25856,9 +26235,13 @@
       <c r="C79" s="10" t="s">
         <v>972</v>
       </c>
-      <c r="D79" s="42"/>
-    </row>
-    <row r="80" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D79" s="57" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E79"/>
+      <c r="F79" s="42"/>
+    </row>
+    <row r="80" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A80" s="1" t="s">
         <v>887</v>
       </c>
@@ -25868,9 +26251,13 @@
       <c r="C80" s="20" t="s">
         <v>905</v>
       </c>
-      <c r="D80" s="42"/>
-    </row>
-    <row r="81" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D80" s="57" t="s">
+        <v>905</v>
+      </c>
+      <c r="E80"/>
+      <c r="F80" s="42"/>
+    </row>
+    <row r="81" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A81" s="1" t="s">
         <v>888</v>
       </c>
@@ -25880,9 +26267,13 @@
       <c r="C81" s="20" t="s">
         <v>922</v>
       </c>
-      <c r="D81" s="42"/>
-    </row>
-    <row r="82" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D81" s="57" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E81"/>
+      <c r="F81" s="42"/>
+    </row>
+    <row r="82" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A82" s="1" t="s">
         <v>890</v>
       </c>
@@ -25892,9 +26283,13 @@
       <c r="C82" s="29" t="s">
         <v>917</v>
       </c>
-      <c r="D82" s="42"/>
-    </row>
-    <row r="83" spans="1:5" s="13" customFormat="1" ht="15">
+      <c r="D82" s="57" t="s">
+        <v>1032</v>
+      </c>
+      <c r="E82"/>
+      <c r="F82" s="42"/>
+    </row>
+    <row r="83" spans="1:7" s="13" customFormat="1" ht="15">
       <c r="A83" s="25" t="s">
         <v>980</v>
       </c>
@@ -25904,17 +26299,26 @@
       <c r="C83" s="29" t="s">
         <v>903</v>
       </c>
-      <c r="D83" s="42"/>
-    </row>
-    <row r="84" spans="1:5" s="42" customFormat="1">
+      <c r="D83" s="57" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E83"/>
+      <c r="F83" s="42" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" s="42" customFormat="1">
       <c r="A84"/>
       <c r="B84" s="7"/>
       <c r="C84"/>
-      <c r="E84" s="13"/>
+      <c r="D84"/>
+      <c r="E84"/>
+      <c r="G84" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
he aclarado los codigos de las correspondencias del SIOSE
</commit_message>
<xml_diff>
--- a/Correspondencias_SIOSE - modificada (v2).xlsx
+++ b/Correspondencias_SIOSE - modificada (v2).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Correspondencias_SIOSE (2)" sheetId="10" r:id="rId1"/>
@@ -3217,7 +3217,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3347,8 +3347,22 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Open Sans"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3371,6 +3385,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -3543,10 +3563,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3637,8 +3658,15 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="60% - Énfasis1" xfId="1" builtinId="32"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
@@ -24960,7 +24988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D38" sqref="D38:D39"/>
     </sheetView>
   </sheetViews>
@@ -26326,10 +26354,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="N2" sqref="N2:N252"/>
-      <selection pane="bottomLeft" activeCell="B219" sqref="B219"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -26376,7 +26404,7 @@
       <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="59" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -26407,7 +26435,7 @@
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="1">
+      <c r="M2" s="58">
         <v>999</v>
       </c>
       <c r="N2" s="1" t="s">
@@ -26438,7 +26466,7 @@
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="1">
+      <c r="M3" s="58">
         <v>165</v>
       </c>
       <c r="N3" s="1" t="s">
@@ -26482,7 +26510,7 @@
       <c r="L4" s="3">
         <v>111</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="58">
         <v>125</v>
       </c>
       <c r="N4" s="1" t="s">
@@ -26526,7 +26554,7 @@
       <c r="L5" s="3">
         <v>111</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5" s="58">
         <v>129</v>
       </c>
       <c r="N5" s="1" t="s">
@@ -26570,7 +26598,7 @@
       <c r="L6" s="3">
         <v>111</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="58">
         <v>130</v>
       </c>
       <c r="N6" s="1" t="s">
@@ -26614,7 +26642,7 @@
       <c r="L7" s="3">
         <v>111</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="58">
         <v>132</v>
       </c>
       <c r="N7" s="1" t="s">
@@ -26658,7 +26686,7 @@
       <c r="L8" s="3">
         <v>111</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8" s="58">
         <v>134</v>
       </c>
       <c r="N8" s="1" t="s">
@@ -26702,7 +26730,7 @@
       <c r="L9" s="3">
         <v>111</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M9" s="58">
         <v>169</v>
       </c>
       <c r="N9" s="1" t="s">
@@ -26746,7 +26774,7 @@
       <c r="L10" s="3">
         <v>111</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M10" s="58">
         <v>170</v>
       </c>
       <c r="N10" s="1" t="s">
@@ -26790,7 +26818,7 @@
       <c r="L11" s="3">
         <v>111</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="58">
         <v>171</v>
       </c>
       <c r="N11" s="1" t="s">
@@ -26834,7 +26862,7 @@
       <c r="L12" s="3">
         <v>111</v>
       </c>
-      <c r="M12" s="1">
+      <c r="M12" s="58">
         <v>936</v>
       </c>
       <c r="N12" s="1" t="s">
@@ -26878,7 +26906,7 @@
       <c r="L13" s="3">
         <v>111</v>
       </c>
-      <c r="M13" s="1">
+      <c r="M13" s="58">
         <v>101</v>
       </c>
       <c r="N13" s="1" t="s">
@@ -26922,7 +26950,7 @@
       <c r="L14" s="3">
         <v>111</v>
       </c>
-      <c r="M14" s="1">
+      <c r="M14" s="58">
         <v>2000</v>
       </c>
       <c r="N14" s="1" t="s">
@@ -26953,6 +26981,7 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="3"/>
+      <c r="M15" s="58"/>
     </row>
     <row r="16" spans="1:14" ht="13.5" customHeight="1">
       <c r="A16" s="1" t="s">
@@ -26991,7 +27020,7 @@
       <c r="L16" s="3">
         <v>112</v>
       </c>
-      <c r="M16" s="1">
+      <c r="M16" s="58">
         <v>2002</v>
       </c>
       <c r="N16" s="1" t="s">
@@ -27035,7 +27064,7 @@
       <c r="L17" s="3">
         <v>112</v>
       </c>
-      <c r="M17" s="1">
+      <c r="M17" s="58">
         <v>117</v>
       </c>
       <c r="N17" s="1" t="s">
@@ -27066,6 +27095,7 @@
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="3"/>
+      <c r="M18" s="58"/>
     </row>
     <row r="19" spans="1:14" ht="13.5" customHeight="1">
       <c r="A19" s="1" t="s">
@@ -27104,7 +27134,7 @@
       <c r="L19" s="3">
         <v>121</v>
       </c>
-      <c r="M19" s="1">
+      <c r="M19" s="58">
         <v>203</v>
       </c>
       <c r="N19" s="1" t="s">
@@ -27148,7 +27178,7 @@
       <c r="L20" s="3">
         <v>121</v>
       </c>
-      <c r="M20" s="1">
+      <c r="M20" s="58">
         <v>222</v>
       </c>
       <c r="N20" s="1" t="s">
@@ -27192,7 +27222,7 @@
       <c r="L21" s="3">
         <v>121</v>
       </c>
-      <c r="M21" s="1">
+      <c r="M21" s="58">
         <v>122</v>
       </c>
       <c r="N21" s="1" t="s">
@@ -27236,7 +27266,7 @@
       <c r="L22" s="3">
         <v>121</v>
       </c>
-      <c r="M22" s="1">
+      <c r="M22" s="58">
         <v>118</v>
       </c>
       <c r="N22" s="1" t="s">
@@ -27280,7 +27310,7 @@
       <c r="L23" s="3">
         <v>121</v>
       </c>
-      <c r="M23" s="1">
+      <c r="M23" s="58">
         <v>119</v>
       </c>
       <c r="N23" s="1" t="s">
@@ -27324,7 +27354,7 @@
       <c r="L24" s="3">
         <v>121</v>
       </c>
-      <c r="M24" s="1">
+      <c r="M24" s="58">
         <v>120</v>
       </c>
       <c r="N24" s="1" t="s">
@@ -27368,7 +27398,7 @@
       <c r="L25" s="3">
         <v>121</v>
       </c>
-      <c r="M25" s="1">
+      <c r="M25" s="58">
         <v>168</v>
       </c>
       <c r="N25" s="1" t="s">
@@ -27399,6 +27429,7 @@
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="3"/>
+      <c r="M26" s="58"/>
     </row>
     <row r="27" spans="1:14" ht="13.5" customHeight="1">
       <c r="A27" s="1" t="s">
@@ -27437,7 +27468,7 @@
       <c r="L27" s="3">
         <v>122</v>
       </c>
-      <c r="M27" s="1">
+      <c r="M27" s="58">
         <v>131</v>
       </c>
       <c r="N27" s="1" t="s">
@@ -27481,7 +27512,7 @@
       <c r="L28" s="3">
         <v>122</v>
       </c>
-      <c r="M28" s="1">
+      <c r="M28" s="58">
         <v>182</v>
       </c>
       <c r="N28" s="1" t="s">
@@ -27525,7 +27556,7 @@
       <c r="L29" s="3">
         <v>122</v>
       </c>
-      <c r="M29" s="1">
+      <c r="M29" s="58">
         <v>184</v>
       </c>
       <c r="N29" s="1" t="s">
@@ -27569,7 +27600,7 @@
       <c r="L30" s="3">
         <v>122</v>
       </c>
-      <c r="M30" s="1">
+      <c r="M30" s="58">
         <v>2004</v>
       </c>
       <c r="N30" s="1" t="s">
@@ -27613,7 +27644,7 @@
       <c r="L31" s="3">
         <v>122</v>
       </c>
-      <c r="M31" s="1">
+      <c r="M31" s="58">
         <v>133</v>
       </c>
       <c r="N31" s="1" t="s">
@@ -27657,7 +27688,7 @@
       <c r="L32" s="3">
         <v>123</v>
       </c>
-      <c r="M32" s="1">
+      <c r="M32" s="58">
         <v>127</v>
       </c>
       <c r="N32" s="1" t="s">
@@ -27701,7 +27732,7 @@
       <c r="L33" s="3">
         <v>123</v>
       </c>
-      <c r="M33" s="1">
+      <c r="M33" s="58">
         <v>128</v>
       </c>
       <c r="N33" s="1" t="s">
@@ -27745,7 +27776,7 @@
       <c r="L34" s="3">
         <v>123</v>
       </c>
-      <c r="M34" s="1">
+      <c r="M34" s="58">
         <v>156</v>
       </c>
       <c r="N34" s="1" t="s">
@@ -27789,7 +27820,7 @@
       <c r="L35" s="3">
         <v>124</v>
       </c>
-      <c r="M35" s="1">
+      <c r="M35" s="58">
         <v>137</v>
       </c>
       <c r="N35" s="1" t="s">
@@ -27833,7 +27864,7 @@
       <c r="L36" s="3">
         <v>124</v>
       </c>
-      <c r="M36" s="1">
+      <c r="M36" s="58">
         <v>1700</v>
       </c>
       <c r="N36" s="1" t="s">
@@ -27877,7 +27908,7 @@
       <c r="L37" s="3">
         <v>122</v>
       </c>
-      <c r="M37" s="1">
+      <c r="M37" s="58">
         <v>113</v>
       </c>
       <c r="N37" s="1" t="s">
@@ -27921,7 +27952,7 @@
       <c r="L38" s="3">
         <v>122</v>
       </c>
-      <c r="M38" s="1">
+      <c r="M38" s="58">
         <v>145</v>
       </c>
       <c r="N38" s="1" t="s">
@@ -27965,7 +27996,7 @@
       <c r="L39" s="3">
         <v>122</v>
       </c>
-      <c r="M39" s="1">
+      <c r="M39" s="58">
         <v>146</v>
       </c>
       <c r="N39" s="1" t="s">
@@ -28009,7 +28040,7 @@
       <c r="L40" s="3">
         <v>122</v>
       </c>
-      <c r="M40" s="1">
+      <c r="M40" s="58">
         <v>147</v>
       </c>
       <c r="N40" s="1" t="s">
@@ -28053,7 +28084,7 @@
       <c r="L41" s="3">
         <v>122</v>
       </c>
-      <c r="M41" s="1">
+      <c r="M41" s="58">
         <v>148</v>
       </c>
       <c r="N41" s="1" t="s">
@@ -28097,7 +28128,7 @@
       <c r="L42" s="3">
         <v>122</v>
       </c>
-      <c r="M42" s="1">
+      <c r="M42" s="58">
         <v>149</v>
       </c>
       <c r="N42" s="1" t="s">
@@ -28141,7 +28172,7 @@
       <c r="L43" s="3">
         <v>122</v>
       </c>
-      <c r="M43" s="1">
+      <c r="M43" s="58">
         <v>150</v>
       </c>
       <c r="N43" s="1" t="s">
@@ -28185,7 +28216,7 @@
       <c r="L44" s="3">
         <v>122</v>
       </c>
-      <c r="M44" s="1">
+      <c r="M44" s="58">
         <v>152</v>
       </c>
       <c r="N44" s="1" t="s">
@@ -28229,7 +28260,7 @@
       <c r="L45" s="3">
         <v>122</v>
       </c>
-      <c r="M45" s="1">
+      <c r="M45" s="58">
         <v>154</v>
       </c>
       <c r="N45" s="1" t="s">
@@ -28273,7 +28304,7 @@
       <c r="L46" s="3">
         <v>122</v>
       </c>
-      <c r="M46" s="1">
+      <c r="M46" s="58">
         <v>159</v>
       </c>
       <c r="N46" s="1" t="s">
@@ -28317,7 +28348,7 @@
       <c r="L47" s="3">
         <v>122</v>
       </c>
-      <c r="M47" s="1">
+      <c r="M47" s="58">
         <v>160</v>
       </c>
       <c r="N47" s="1" t="s">
@@ -28361,7 +28392,7 @@
       <c r="L48" s="3">
         <v>122</v>
       </c>
-      <c r="M48" s="1">
+      <c r="M48" s="58">
         <v>162</v>
       </c>
       <c r="N48" s="1" t="s">
@@ -28405,7 +28436,7 @@
       <c r="L49" s="3">
         <v>122</v>
       </c>
-      <c r="M49" s="1">
+      <c r="M49" s="58">
         <v>164</v>
       </c>
       <c r="N49" s="1" t="s">
@@ -28449,7 +28480,7 @@
       <c r="L50" s="3">
         <v>122</v>
       </c>
-      <c r="M50" s="1">
+      <c r="M50" s="58">
         <v>174</v>
       </c>
       <c r="N50" s="1" t="s">
@@ -28493,7 +28524,7 @@
       <c r="L51" s="3">
         <v>122</v>
       </c>
-      <c r="M51" s="1">
+      <c r="M51" s="58">
         <v>175</v>
       </c>
       <c r="N51" s="1" t="s">
@@ -28537,7 +28568,7 @@
       <c r="L52" s="3">
         <v>122</v>
       </c>
-      <c r="M52" s="1">
+      <c r="M52" s="58">
         <v>176</v>
       </c>
       <c r="N52" s="1" t="s">
@@ -28581,7 +28612,7 @@
       <c r="L53" s="3">
         <v>122</v>
       </c>
-      <c r="M53" s="1">
+      <c r="M53" s="58">
         <v>181</v>
       </c>
       <c r="N53" s="1" t="s">
@@ -28612,6 +28643,7 @@
       </c>
       <c r="K54" s="2"/>
       <c r="L54" s="3"/>
+      <c r="M54" s="58"/>
     </row>
     <row r="55" spans="1:14" ht="13.5" customHeight="1">
       <c r="A55" s="1" t="s">
@@ -28650,7 +28682,7 @@
       <c r="L55" s="3">
         <v>131</v>
       </c>
-      <c r="M55" s="1">
+      <c r="M55" s="58">
         <v>346</v>
       </c>
       <c r="N55" s="1" t="s">
@@ -28694,7 +28726,7 @@
       <c r="L56" s="3">
         <v>131</v>
       </c>
-      <c r="M56" s="1">
+      <c r="M56" s="58">
         <v>151</v>
       </c>
       <c r="N56" s="1" t="s">
@@ -28738,7 +28770,7 @@
       <c r="L57" s="3">
         <v>131</v>
       </c>
-      <c r="M57" s="1">
+      <c r="M57" s="58">
         <v>2007</v>
       </c>
       <c r="N57" s="1" t="s">
@@ -28782,7 +28814,7 @@
       <c r="L58" s="3">
         <v>132</v>
       </c>
-      <c r="M58" s="1">
+      <c r="M58" s="58">
         <v>153</v>
       </c>
       <c r="N58" s="1" t="s">
@@ -28826,6 +28858,7 @@
       <c r="L59" s="3">
         <v>133</v>
       </c>
+      <c r="M59" s="58"/>
     </row>
     <row r="60" spans="1:14" ht="13.5" customHeight="1">
       <c r="A60" s="1" t="s">
@@ -28864,7 +28897,7 @@
       <c r="L60" s="3">
         <v>132</v>
       </c>
-      <c r="M60" s="1">
+      <c r="M60" s="58">
         <v>157</v>
       </c>
       <c r="N60" s="1" t="s">
@@ -28895,6 +28928,7 @@
       </c>
       <c r="K61" s="2"/>
       <c r="L61" s="3"/>
+      <c r="M61" s="58"/>
     </row>
     <row r="62" spans="1:14" ht="13.5" customHeight="1">
       <c r="A62" s="1" t="s">
@@ -28933,7 +28967,7 @@
       <c r="L62" s="3">
         <v>141</v>
       </c>
-      <c r="M62" s="1">
+      <c r="M62" s="58">
         <v>123</v>
       </c>
       <c r="N62" s="1" t="s">
@@ -28977,7 +29011,7 @@
       <c r="L63" s="3">
         <v>141</v>
       </c>
-      <c r="M63" s="1">
+      <c r="M63" s="58">
         <v>177</v>
       </c>
       <c r="N63" s="1" t="s">
@@ -29021,7 +29055,7 @@
       <c r="L64" s="3">
         <v>141</v>
       </c>
-      <c r="M64" s="1">
+      <c r="M64" s="58">
         <v>2005</v>
       </c>
       <c r="N64" s="1" t="s">
@@ -29065,7 +29099,7 @@
       <c r="L65" s="3">
         <v>141</v>
       </c>
-      <c r="M65" s="1">
+      <c r="M65" s="58">
         <v>180</v>
       </c>
       <c r="N65" s="1" t="s">
@@ -29109,7 +29143,7 @@
       <c r="L66" s="3">
         <v>141</v>
       </c>
-      <c r="M66" s="1">
+      <c r="M66" s="58">
         <v>158</v>
       </c>
       <c r="N66" s="1" t="s">
@@ -29153,7 +29187,7 @@
       <c r="L67" s="3">
         <v>142</v>
       </c>
-      <c r="M67" s="1">
+      <c r="M67" s="58">
         <v>102</v>
       </c>
       <c r="N67" s="1" t="s">
@@ -29197,7 +29231,7 @@
       <c r="L68" s="3">
         <v>142</v>
       </c>
-      <c r="M68" s="1">
+      <c r="M68" s="58">
         <v>105</v>
       </c>
       <c r="N68" s="1" t="s">
@@ -29241,7 +29275,7 @@
       <c r="L69" s="3">
         <v>142</v>
       </c>
-      <c r="M69" s="1">
+      <c r="M69" s="58">
         <v>106</v>
       </c>
       <c r="N69" s="1" t="s">
@@ -29285,7 +29319,7 @@
       <c r="L70" s="3">
         <v>142</v>
       </c>
-      <c r="M70" s="1">
+      <c r="M70" s="58">
         <v>107</v>
       </c>
       <c r="N70" s="1" t="s">
@@ -29329,7 +29363,7 @@
       <c r="L71" s="3">
         <v>142</v>
       </c>
-      <c r="M71" s="1">
+      <c r="M71" s="58">
         <v>108</v>
       </c>
       <c r="N71" s="1" t="s">
@@ -29373,7 +29407,7 @@
       <c r="L72" s="3">
         <v>142</v>
       </c>
-      <c r="M72" s="1">
+      <c r="M72" s="58">
         <v>173</v>
       </c>
       <c r="N72" s="1" t="s">
@@ -29417,7 +29451,7 @@
       <c r="L73" s="3">
         <v>142</v>
       </c>
-      <c r="M73" s="1">
+      <c r="M73" s="58">
         <v>138</v>
       </c>
       <c r="N73" s="1" t="s">
@@ -29461,7 +29495,7 @@
       <c r="L74" s="3">
         <v>142</v>
       </c>
-      <c r="M74" s="1">
+      <c r="M74" s="58">
         <v>139</v>
       </c>
       <c r="N74" s="1" t="s">
@@ -29505,7 +29539,7 @@
       <c r="L75" s="3">
         <v>142</v>
       </c>
-      <c r="M75" s="1">
+      <c r="M75" s="58">
         <v>140</v>
       </c>
       <c r="N75" s="1" t="s">
@@ -29549,7 +29583,7 @@
       <c r="L76" s="3">
         <v>142</v>
       </c>
-      <c r="M76" s="1">
+      <c r="M76" s="58">
         <v>142</v>
       </c>
       <c r="N76" s="1" t="s">
@@ -29593,7 +29627,7 @@
       <c r="L77" s="3">
         <v>142</v>
       </c>
-      <c r="M77" s="1">
+      <c r="M77" s="58">
         <v>144</v>
       </c>
       <c r="N77" s="1" t="s">
@@ -29637,7 +29671,7 @@
       <c r="L78" s="3">
         <v>142</v>
       </c>
-      <c r="M78" s="1">
+      <c r="M78" s="58">
         <v>135</v>
       </c>
       <c r="N78" s="1" t="s">
@@ -29681,7 +29715,7 @@
       <c r="L79" s="3">
         <v>142</v>
       </c>
-      <c r="M79" s="1">
+      <c r="M79" s="58">
         <v>136</v>
       </c>
       <c r="N79" s="1" t="s">
@@ -29725,7 +29759,7 @@
       <c r="L80" s="3">
         <v>142</v>
       </c>
-      <c r="M80" s="1">
+      <c r="M80" s="58">
         <v>143</v>
       </c>
       <c r="N80" s="1" t="s">
@@ -29769,7 +29803,7 @@
       <c r="L81" s="3">
         <v>142</v>
       </c>
-      <c r="M81" s="1">
+      <c r="M81" s="58">
         <v>172</v>
       </c>
       <c r="N81" s="1" t="s">
@@ -29813,7 +29847,7 @@
       <c r="L82" s="3">
         <v>142</v>
       </c>
-      <c r="M82" s="1">
+      <c r="M82" s="58">
         <v>124</v>
       </c>
       <c r="N82" s="1" t="s">
@@ -29844,6 +29878,7 @@
       </c>
       <c r="K83" s="2"/>
       <c r="L83" s="3"/>
+      <c r="M83" s="58"/>
     </row>
     <row r="84" spans="1:14" ht="13.5" customHeight="1">
       <c r="A84" s="1" t="s">
@@ -29869,6 +29904,7 @@
       </c>
       <c r="K84" s="2"/>
       <c r="L84" s="3"/>
+      <c r="M84" s="58"/>
     </row>
     <row r="85" spans="1:14" ht="13.5" customHeight="1">
       <c r="A85" s="1" t="s">
@@ -29894,6 +29930,7 @@
       </c>
       <c r="K85" s="2"/>
       <c r="L85" s="3"/>
+      <c r="M85" s="58"/>
     </row>
     <row r="86" spans="1:14" ht="13.5" customHeight="1">
       <c r="A86" s="1" t="s">
@@ -29919,7 +29956,7 @@
       </c>
       <c r="K86" s="2"/>
       <c r="L86" s="3"/>
-      <c r="M86" s="1">
+      <c r="M86" s="58">
         <v>210</v>
       </c>
       <c r="N86" s="1" t="s">
@@ -29963,6 +30000,7 @@
       <c r="L87" s="3">
         <v>421</v>
       </c>
+      <c r="M87" s="58"/>
     </row>
     <row r="88" spans="1:14" ht="13.5" customHeight="1">
       <c r="A88" s="1" t="s">
@@ -30001,6 +30039,7 @@
       <c r="L88" s="3">
         <v>421</v>
       </c>
+      <c r="M88" s="58"/>
     </row>
     <row r="89" spans="1:14" ht="13.5" customHeight="1">
       <c r="A89" s="1" t="s">
@@ -30039,7 +30078,7 @@
       <c r="L89" s="3">
         <v>421</v>
       </c>
-      <c r="M89" s="1">
+      <c r="M89" s="58">
         <v>217</v>
       </c>
       <c r="N89" s="1" t="s">
@@ -30070,6 +30109,7 @@
       </c>
       <c r="K90" s="2"/>
       <c r="L90" s="3"/>
+      <c r="M90" s="58"/>
     </row>
     <row r="91" spans="1:14" ht="13.5" customHeight="1">
       <c r="A91" s="1" t="s">
@@ -30108,7 +30148,7 @@
       <c r="L91" s="3">
         <v>422</v>
       </c>
-      <c r="M91" s="1">
+      <c r="M91" s="58">
         <v>221</v>
       </c>
       <c r="N91" s="1" t="s">
@@ -30152,6 +30192,7 @@
       <c r="L92" s="3">
         <v>422</v>
       </c>
+      <c r="M92" s="58"/>
     </row>
     <row r="93" spans="1:14" ht="13.5" customHeight="1">
       <c r="A93" s="1" t="s">
@@ -30190,7 +30231,7 @@
       <c r="L93" s="3">
         <v>422</v>
       </c>
-      <c r="M93" s="1">
+      <c r="M93" s="58">
         <v>231</v>
       </c>
       <c r="N93" s="1" t="s">
@@ -30234,7 +30275,7 @@
       <c r="L94" s="3">
         <v>522</v>
       </c>
-      <c r="M94" s="1">
+      <c r="M94" s="58">
         <v>241</v>
       </c>
       <c r="N94" s="1" t="s">
@@ -30278,7 +30319,7 @@
       <c r="L95" s="3">
         <v>523</v>
       </c>
-      <c r="M95" s="1">
+      <c r="M95" s="58">
         <v>291</v>
       </c>
       <c r="N95" s="1" t="s">
@@ -30309,6 +30350,7 @@
       </c>
       <c r="K96" s="2"/>
       <c r="L96" s="3"/>
+      <c r="M96" s="58"/>
     </row>
     <row r="97" spans="1:14" ht="13.5" customHeight="1">
       <c r="A97" s="1" t="s">
@@ -30334,7 +30376,7 @@
       </c>
       <c r="K97" s="2"/>
       <c r="L97" s="3"/>
-      <c r="M97" s="1">
+      <c r="M97" s="58">
         <v>310</v>
       </c>
       <c r="N97" s="1" t="s">
@@ -30365,7 +30407,7 @@
       </c>
       <c r="K98" s="2"/>
       <c r="L98" s="3"/>
-      <c r="M98" s="1">
+      <c r="M98" s="58">
         <v>960</v>
       </c>
       <c r="N98" s="1" t="s">
@@ -30409,7 +30451,7 @@
       <c r="L99" s="3">
         <v>511</v>
       </c>
-      <c r="M99" s="1">
+      <c r="M99" s="58">
         <v>318</v>
       </c>
       <c r="N99" s="1" t="s">
@@ -30440,6 +30482,7 @@
       </c>
       <c r="K100" s="2"/>
       <c r="L100" s="3"/>
+      <c r="M100" s="58"/>
     </row>
     <row r="101" spans="1:14" ht="13.5" customHeight="1">
       <c r="A101" s="1" t="s">
@@ -30478,7 +30521,7 @@
       <c r="L101" s="3">
         <v>511</v>
       </c>
-      <c r="M101" s="1">
+      <c r="M101" s="58">
         <v>315</v>
       </c>
       <c r="N101" s="1" t="s">
@@ -30522,7 +30565,7 @@
       <c r="L102" s="3">
         <v>511</v>
       </c>
-      <c r="M102" s="1">
+      <c r="M102" s="58">
         <v>317</v>
       </c>
       <c r="N102" s="1" t="s">
@@ -30566,7 +30609,7 @@
       <c r="L103" s="3">
         <v>511</v>
       </c>
-      <c r="M103" s="1">
+      <c r="M103" s="58">
         <v>2008</v>
       </c>
       <c r="N103" s="1" t="s">
@@ -30610,7 +30653,7 @@
       <c r="L104" s="3">
         <v>511</v>
       </c>
-      <c r="M104" s="1">
+      <c r="M104" s="58">
         <v>319</v>
       </c>
       <c r="N104" s="1" t="s">
@@ -30654,7 +30697,7 @@
       <c r="L105" s="3">
         <v>511</v>
       </c>
-      <c r="M105" s="1">
+      <c r="M105" s="58">
         <v>200</v>
       </c>
       <c r="N105" s="1" t="s">
@@ -30698,7 +30741,7 @@
       <c r="L106" s="3">
         <v>511</v>
       </c>
-      <c r="M106" s="1">
+      <c r="M106" s="58">
         <v>201</v>
       </c>
       <c r="N106" s="1" t="s">
@@ -30742,7 +30785,7 @@
       <c r="L107" s="3">
         <v>511</v>
       </c>
-      <c r="M107" s="1">
+      <c r="M107" s="58">
         <v>332</v>
       </c>
       <c r="N107" s="1" t="s">
@@ -30773,6 +30816,7 @@
       </c>
       <c r="K108" s="2"/>
       <c r="L108" s="3"/>
+      <c r="M108" s="58"/>
     </row>
     <row r="109" spans="1:14" ht="13.5" customHeight="1">
       <c r="A109" s="1" t="s">
@@ -30811,7 +30855,7 @@
       <c r="L109" s="3">
         <v>512</v>
       </c>
-      <c r="M109" s="1">
+      <c r="M109" s="58">
         <v>341</v>
       </c>
       <c r="N109" s="1" t="s">
@@ -30855,7 +30899,7 @@
       <c r="L110" s="3">
         <v>512</v>
       </c>
-      <c r="M110" s="1">
+      <c r="M110" s="58">
         <v>345</v>
       </c>
       <c r="N110" s="1" t="s">
@@ -30886,6 +30930,7 @@
       </c>
       <c r="K111" s="2"/>
       <c r="L111" s="3"/>
+      <c r="M111" s="58"/>
     </row>
     <row r="112" spans="1:14" ht="13.5" customHeight="1">
       <c r="A112" s="1" t="s">
@@ -30911,7 +30956,7 @@
       </c>
       <c r="K112" s="2"/>
       <c r="L112" s="3"/>
-      <c r="M112" s="1">
+      <c r="M112" s="58">
         <v>405</v>
       </c>
       <c r="N112" s="1" t="s">
@@ -30942,6 +30987,7 @@
       </c>
       <c r="K113" s="2"/>
       <c r="L113" s="3"/>
+      <c r="M113" s="58"/>
     </row>
     <row r="114" spans="1:14" ht="13.5" customHeight="1">
       <c r="A114" s="1" t="s">
@@ -30980,6 +31026,7 @@
       <c r="L114" s="3">
         <v>211</v>
       </c>
+      <c r="M114" s="58"/>
     </row>
     <row r="115" spans="1:14" ht="13.5" customHeight="1">
       <c r="A115" s="1" t="s">
@@ -31005,6 +31052,7 @@
       </c>
       <c r="K115" s="2"/>
       <c r="L115" s="3"/>
+      <c r="M115" s="58"/>
     </row>
     <row r="116" spans="1:14" ht="13.5" customHeight="1">
       <c r="A116" s="1" t="s">
@@ -31043,7 +31091,7 @@
       <c r="L116" s="3">
         <v>223</v>
       </c>
-      <c r="M116" s="1">
+      <c r="M116" s="58">
         <v>416</v>
       </c>
       <c r="N116" s="1" t="s">
@@ -31087,7 +31135,7 @@
       <c r="L117" s="3">
         <v>221</v>
       </c>
-      <c r="M117" s="1">
+      <c r="M117" s="58">
         <v>417</v>
       </c>
       <c r="N117" s="1" t="s">
@@ -31131,7 +31179,7 @@
       <c r="L118" s="3">
         <v>222</v>
       </c>
-      <c r="M118" s="1">
+      <c r="M118" s="58">
         <v>460</v>
       </c>
       <c r="N118" s="1" t="s">
@@ -31162,6 +31210,7 @@
       </c>
       <c r="K119" s="2"/>
       <c r="L119" s="3"/>
+      <c r="M119" s="58"/>
     </row>
     <row r="120" spans="1:14" ht="13.5" customHeight="1">
       <c r="A120" s="1" t="s">
@@ -31187,6 +31236,7 @@
       </c>
       <c r="K120" s="2"/>
       <c r="L120" s="3"/>
+      <c r="M120" s="58"/>
     </row>
     <row r="121" spans="1:14" ht="13.5" customHeight="1">
       <c r="A121" s="1" t="s">
@@ -31212,6 +31262,7 @@
       </c>
       <c r="K121" s="2"/>
       <c r="L121" s="3"/>
+      <c r="M121" s="58"/>
     </row>
     <row r="122" spans="1:14" ht="13.5" customHeight="1">
       <c r="A122" s="1" t="s">
@@ -31250,7 +31301,7 @@
       <c r="L122" s="3">
         <v>212</v>
       </c>
-      <c r="M122" s="1">
+      <c r="M122" s="58">
         <v>421</v>
       </c>
       <c r="N122" s="1" t="s">
@@ -31294,7 +31345,7 @@
       <c r="L123" s="3">
         <v>212</v>
       </c>
-      <c r="M123" s="1">
+      <c r="M123" s="58">
         <v>403</v>
       </c>
       <c r="N123" s="1" t="s">
@@ -31338,7 +31389,7 @@
       <c r="L124" s="3">
         <v>212</v>
       </c>
-      <c r="M124" s="1">
+      <c r="M124" s="58">
         <v>404</v>
       </c>
       <c r="N124" s="1" t="s">
@@ -31382,6 +31433,7 @@
       <c r="L125" s="3">
         <v>212</v>
       </c>
+      <c r="M125" s="58"/>
     </row>
     <row r="126" spans="1:14" ht="13.5" customHeight="1">
       <c r="A126" s="1" t="s">
@@ -31420,6 +31472,7 @@
       <c r="L126" s="3">
         <v>212</v>
       </c>
+      <c r="M126" s="58"/>
     </row>
     <row r="127" spans="1:14" ht="13.5" customHeight="1">
       <c r="A127" s="1" t="s">
@@ -31458,6 +31511,7 @@
       <c r="L127" s="3">
         <v>212</v>
       </c>
+      <c r="M127" s="58"/>
     </row>
     <row r="128" spans="1:14" ht="13.5" customHeight="1">
       <c r="A128" s="1" t="s">
@@ -31483,6 +31537,7 @@
       </c>
       <c r="K128" s="2"/>
       <c r="L128" s="3"/>
+      <c r="M128" s="58"/>
     </row>
     <row r="129" spans="1:14" ht="13.5" customHeight="1">
       <c r="A129" s="1" t="s">
@@ -31521,6 +31576,7 @@
       <c r="L129" s="3">
         <v>212</v>
       </c>
+      <c r="M129" s="58"/>
     </row>
     <row r="130" spans="1:14" ht="13.5" customHeight="1">
       <c r="A130" s="1" t="s">
@@ -31546,6 +31602,7 @@
       </c>
       <c r="K130" s="2"/>
       <c r="L130" s="3"/>
+      <c r="M130" s="58"/>
     </row>
     <row r="131" spans="1:14" ht="13.5" customHeight="1">
       <c r="A131" s="1" t="s">
@@ -31584,6 +31641,7 @@
       <c r="L131" s="3">
         <v>212</v>
       </c>
+      <c r="M131" s="58"/>
     </row>
     <row r="132" spans="1:14" ht="13.5" customHeight="1">
       <c r="A132" s="1" t="s">
@@ -31622,7 +31680,7 @@
       <c r="L132" s="3">
         <v>212</v>
       </c>
-      <c r="M132" s="1">
+      <c r="M132" s="58">
         <v>435</v>
       </c>
       <c r="N132" s="1" t="s">
@@ -31666,7 +31724,7 @@
       <c r="L133" s="3">
         <v>212</v>
       </c>
-      <c r="M133" s="1">
+      <c r="M133" s="58">
         <v>989</v>
       </c>
       <c r="N133" s="1" t="s">
@@ -31710,7 +31768,7 @@
       <c r="L134" s="3">
         <v>212</v>
       </c>
-      <c r="M134" s="1">
+      <c r="M134" s="58">
         <v>997</v>
       </c>
       <c r="N134" s="1" t="s">
@@ -31754,7 +31812,7 @@
       <c r="L135" s="3">
         <v>212</v>
       </c>
-      <c r="M135" s="1">
+      <c r="M135" s="58">
         <v>961</v>
       </c>
       <c r="N135" s="1" t="s">
@@ -31798,7 +31856,7 @@
       <c r="L136" s="3">
         <v>212</v>
       </c>
-      <c r="M136" s="1">
+      <c r="M136" s="58">
         <v>962</v>
       </c>
       <c r="N136" s="1" t="s">
@@ -31842,7 +31900,7 @@
       <c r="L137" s="3">
         <v>212</v>
       </c>
-      <c r="M137" s="1">
+      <c r="M137" s="58">
         <v>431</v>
       </c>
       <c r="N137" s="1" t="s">
@@ -31873,7 +31931,7 @@
       </c>
       <c r="K138" s="2"/>
       <c r="L138" s="3"/>
-      <c r="M138" s="1">
+      <c r="M138" s="58">
         <v>410</v>
       </c>
       <c r="N138" s="1" t="s">
@@ -31904,6 +31962,7 @@
       </c>
       <c r="K139" s="2"/>
       <c r="L139" s="3"/>
+      <c r="M139" s="58"/>
     </row>
     <row r="140" spans="1:14" ht="13.5" customHeight="1">
       <c r="A140" s="1" t="s">
@@ -31942,6 +32001,7 @@
       <c r="L140" s="3">
         <v>241</v>
       </c>
+      <c r="M140" s="58"/>
     </row>
     <row r="141" spans="1:14" ht="13.5" customHeight="1">
       <c r="A141" s="1" t="s">
@@ -31967,6 +32027,7 @@
       </c>
       <c r="K141" s="2"/>
       <c r="L141" s="3"/>
+      <c r="M141" s="58"/>
     </row>
     <row r="142" spans="1:14" ht="13.5" customHeight="1">
       <c r="A142" s="1" t="s">
@@ -32005,7 +32066,7 @@
       <c r="L142" s="3">
         <v>242</v>
       </c>
-      <c r="M142" s="1">
+      <c r="M142" s="58">
         <v>445</v>
       </c>
       <c r="N142" s="1" t="s">
@@ -32049,7 +32110,7 @@
       <c r="L143" s="3">
         <v>242</v>
       </c>
-      <c r="M143" s="1">
+      <c r="M143" s="58">
         <v>428</v>
       </c>
       <c r="N143" s="1" t="s">
@@ -32093,7 +32154,7 @@
       <c r="L144" s="3">
         <v>242</v>
       </c>
-      <c r="M144" s="1">
+      <c r="M144" s="58">
         <v>988</v>
       </c>
       <c r="N144" s="1" t="s">
@@ -32137,7 +32198,7 @@
       <c r="L145" s="3">
         <v>242</v>
       </c>
-      <c r="M145" s="1">
+      <c r="M145" s="58">
         <v>965</v>
       </c>
       <c r="N145" s="1" t="s">
@@ -32181,7 +32242,7 @@
       <c r="L146" s="3">
         <v>242</v>
       </c>
-      <c r="M146" s="1">
+      <c r="M146" s="58">
         <v>970</v>
       </c>
       <c r="N146" s="1" t="s">
@@ -32225,7 +32286,7 @@
       <c r="L147" s="3">
         <v>242</v>
       </c>
-      <c r="M147" s="1">
+      <c r="M147" s="58">
         <v>975</v>
       </c>
       <c r="N147" s="1" t="s">
@@ -32269,7 +32330,7 @@
       <c r="L148" s="3">
         <v>242</v>
       </c>
-      <c r="M148" s="1">
+      <c r="M148" s="58">
         <v>979</v>
       </c>
       <c r="N148" s="1" t="s">
@@ -32313,7 +32374,7 @@
       <c r="L149" s="3">
         <v>242</v>
       </c>
-      <c r="M149" s="1">
+      <c r="M149" s="58">
         <v>982</v>
       </c>
       <c r="N149" s="1" t="s">
@@ -32357,7 +32418,7 @@
       <c r="L150" s="3">
         <v>242</v>
       </c>
-      <c r="M150" s="1">
+      <c r="M150" s="58">
         <v>986</v>
       </c>
       <c r="N150" s="1" t="s">
@@ -32391,6 +32452,7 @@
       </c>
       <c r="K151" s="2"/>
       <c r="L151" s="3"/>
+      <c r="M151" s="58"/>
     </row>
     <row r="152" spans="1:14" ht="13.5" customHeight="1">
       <c r="A152" s="1" t="s">
@@ -32416,6 +32478,7 @@
       </c>
       <c r="K152" s="2"/>
       <c r="L152" s="3"/>
+      <c r="M152" s="58"/>
     </row>
     <row r="153" spans="1:14" ht="13.5" customHeight="1">
       <c r="A153" s="1" t="s">
@@ -32454,6 +32517,7 @@
       <c r="L153" s="3">
         <v>242</v>
       </c>
+      <c r="M153" s="58"/>
     </row>
     <row r="154" spans="1:14" ht="13.5" customHeight="1">
       <c r="A154" s="1" t="s">
@@ -32492,6 +32556,7 @@
       <c r="L154" s="3">
         <v>242</v>
       </c>
+      <c r="M154" s="58"/>
     </row>
     <row r="155" spans="1:14" ht="13.5" customHeight="1">
       <c r="A155" s="1" t="s">
@@ -32530,6 +32595,7 @@
       <c r="L155" s="3">
         <v>242</v>
       </c>
+      <c r="M155" s="58"/>
     </row>
     <row r="156" spans="1:14" ht="13.5" customHeight="1">
       <c r="A156" s="1" t="s">
@@ -32568,7 +32634,7 @@
       <c r="L156" s="3">
         <v>242</v>
       </c>
-      <c r="M156" s="1">
+      <c r="M156" s="58">
         <v>973</v>
       </c>
       <c r="N156" s="1" t="s">
@@ -32612,7 +32678,7 @@
       <c r="L157" s="3">
         <v>242</v>
       </c>
-      <c r="M157" s="1">
+      <c r="M157" s="58">
         <v>974</v>
       </c>
       <c r="N157" s="1" t="s">
@@ -32656,7 +32722,7 @@
       <c r="L158" s="3">
         <v>242</v>
       </c>
-      <c r="M158" s="1">
+      <c r="M158" s="58">
         <v>977</v>
       </c>
       <c r="N158" s="1" t="s">
@@ -32700,7 +32766,7 @@
       <c r="L159" s="3">
         <v>242</v>
       </c>
-      <c r="M159" s="1">
+      <c r="M159" s="58">
         <v>978</v>
       </c>
       <c r="N159" s="1" t="s">
@@ -32744,7 +32810,7 @@
       <c r="L160" s="3">
         <v>242</v>
       </c>
-      <c r="M160" s="1">
+      <c r="M160" s="58">
         <v>981</v>
       </c>
       <c r="N160" s="1" t="s">
@@ -32788,7 +32854,7 @@
       <c r="L161" s="3">
         <v>242</v>
       </c>
-      <c r="M161" s="1">
+      <c r="M161" s="58">
         <v>984</v>
       </c>
       <c r="N161" s="1" t="s">
@@ -32819,6 +32885,7 @@
       </c>
       <c r="K162" s="2"/>
       <c r="L162" s="3"/>
+      <c r="M162" s="58"/>
     </row>
     <row r="163" spans="1:14" ht="13.5" customHeight="1">
       <c r="A163" s="1" t="s">
@@ -32857,6 +32924,7 @@
       <c r="L163" s="3">
         <v>242</v>
       </c>
+      <c r="M163" s="58"/>
     </row>
     <row r="164" spans="1:14" ht="13.5" customHeight="1">
       <c r="A164" s="1" t="s">
@@ -32895,6 +32963,7 @@
       <c r="L164" s="3">
         <v>242</v>
       </c>
+      <c r="M164" s="58"/>
     </row>
     <row r="165" spans="1:14" ht="13.5" customHeight="1">
       <c r="A165" s="1" t="s">
@@ -32933,6 +33002,7 @@
       <c r="L165" s="3">
         <v>242</v>
       </c>
+      <c r="M165" s="58"/>
     </row>
     <row r="166" spans="1:14" ht="13.5" customHeight="1">
       <c r="A166" s="1" t="s">
@@ -32971,7 +33041,7 @@
       <c r="L166" s="3">
         <v>242</v>
       </c>
-      <c r="M166" s="1">
+      <c r="M166" s="58">
         <v>963</v>
       </c>
       <c r="N166" s="1" t="s">
@@ -33015,7 +33085,7 @@
       <c r="L167" s="3">
         <v>242</v>
       </c>
-      <c r="M167" s="1">
+      <c r="M167" s="58">
         <v>964</v>
       </c>
       <c r="N167" s="1" t="s">
@@ -33059,7 +33129,7 @@
       <c r="L168" s="3">
         <v>242</v>
       </c>
-      <c r="M168" s="1">
+      <c r="M168" s="58">
         <v>967</v>
       </c>
       <c r="N168" s="1" t="s">
@@ -33103,7 +33173,7 @@
       <c r="L169" s="3">
         <v>242</v>
       </c>
-      <c r="M169" s="1">
+      <c r="M169" s="58">
         <v>968</v>
       </c>
       <c r="N169" s="1" t="s">
@@ -33147,7 +33217,7 @@
       <c r="L170" s="3">
         <v>242</v>
       </c>
-      <c r="M170" s="1">
+      <c r="M170" s="58">
         <v>969</v>
       </c>
       <c r="N170" s="1" t="s">
@@ -33191,7 +33261,7 @@
       <c r="L171" s="3">
         <v>242</v>
       </c>
-      <c r="M171" s="1">
+      <c r="M171" s="58">
         <v>988</v>
       </c>
       <c r="N171" s="1" t="s">
@@ -33235,7 +33305,7 @@
       <c r="L172" s="3">
         <v>242</v>
       </c>
-      <c r="M172" s="1">
+      <c r="M172" s="58">
         <v>989</v>
       </c>
       <c r="N172" s="1" t="s">
@@ -33266,6 +33336,7 @@
       </c>
       <c r="K173" s="2"/>
       <c r="L173" s="3"/>
+      <c r="M173" s="58"/>
     </row>
     <row r="174" spans="1:14" ht="13.5" customHeight="1">
       <c r="A174" s="1" t="s">
@@ -33304,6 +33375,7 @@
       <c r="L174" s="3">
         <v>243</v>
       </c>
+      <c r="M174" s="58"/>
     </row>
     <row r="175" spans="1:14" ht="13.5" customHeight="1">
       <c r="A175" s="1" t="s">
@@ -33342,6 +33414,7 @@
       <c r="L175" s="3">
         <v>243</v>
       </c>
+      <c r="M175" s="58"/>
     </row>
     <row r="176" spans="1:14" ht="13.5" customHeight="1">
       <c r="A176" s="1" t="s">
@@ -33380,6 +33453,7 @@
       <c r="L176" s="3">
         <v>243</v>
       </c>
+      <c r="M176" s="58"/>
     </row>
     <row r="177" spans="1:14" ht="13.5" customHeight="1">
       <c r="A177" s="1" t="s">
@@ -33418,6 +33492,7 @@
       <c r="L177" s="3">
         <v>243</v>
       </c>
+      <c r="M177" s="58"/>
     </row>
     <row r="178" spans="1:14" ht="13.5" customHeight="1">
       <c r="A178" s="1" t="s">
@@ -33456,6 +33531,7 @@
       <c r="L178" s="3">
         <v>243</v>
       </c>
+      <c r="M178" s="58"/>
     </row>
     <row r="179" spans="1:14" ht="13.5" customHeight="1">
       <c r="A179" s="1" t="s">
@@ -33481,6 +33557,7 @@
       </c>
       <c r="K179" s="2"/>
       <c r="L179" s="3"/>
+      <c r="M179" s="58"/>
     </row>
     <row r="180" spans="1:14" ht="13.5" customHeight="1">
       <c r="A180" s="1" t="s">
@@ -33519,6 +33596,7 @@
       <c r="L180" s="3">
         <v>243</v>
       </c>
+      <c r="M180" s="58"/>
     </row>
     <row r="181" spans="1:14" ht="13.5" customHeight="1">
       <c r="A181" s="1" t="s">
@@ -33557,6 +33635,7 @@
       <c r="L181" s="3">
         <v>243</v>
       </c>
+      <c r="M181" s="58"/>
     </row>
     <row r="182" spans="1:14" ht="13.5" customHeight="1">
       <c r="A182" s="1" t="s">
@@ -33582,7 +33661,7 @@
       </c>
       <c r="K182" s="2"/>
       <c r="L182" s="3"/>
-      <c r="M182" s="1">
+      <c r="M182" s="58">
         <v>194</v>
       </c>
       <c r="N182" s="1" t="s">
@@ -33613,6 +33692,7 @@
       </c>
       <c r="K183" s="2"/>
       <c r="L183" s="3"/>
+      <c r="M183" s="58"/>
     </row>
     <row r="184" spans="1:14" ht="13.5" customHeight="1">
       <c r="A184" s="1" t="s">
@@ -33638,6 +33718,7 @@
       </c>
       <c r="K184" s="2"/>
       <c r="L184" s="3"/>
+      <c r="M184" s="58"/>
     </row>
     <row r="185" spans="1:14" ht="13.5" customHeight="1">
       <c r="A185" s="1" t="s">
@@ -33676,7 +33757,7 @@
       <c r="L185" s="3">
         <v>311</v>
       </c>
-      <c r="M185" s="1">
+      <c r="M185" s="58">
         <v>510</v>
       </c>
       <c r="N185" s="1" t="s">
@@ -33720,7 +33801,7 @@
       <c r="L186" s="3">
         <v>312</v>
       </c>
-      <c r="M186" s="1">
+      <c r="M186" s="58">
         <v>520</v>
       </c>
       <c r="N186" s="1" t="s">
@@ -33764,7 +33845,7 @@
       <c r="L187" s="3">
         <v>311</v>
       </c>
-      <c r="M187" s="1">
+      <c r="M187" s="58">
         <v>530</v>
       </c>
       <c r="N187" s="1" t="s">
@@ -33808,7 +33889,7 @@
       <c r="L188" s="3">
         <v>311</v>
       </c>
-      <c r="M188" s="1">
+      <c r="M188" s="58">
         <v>540</v>
       </c>
       <c r="N188" s="1" t="s">
@@ -33852,7 +33933,7 @@
       <c r="L189" s="3">
         <v>313</v>
       </c>
-      <c r="M189" s="1">
+      <c r="M189" s="58">
         <v>550</v>
       </c>
       <c r="N189" s="1" t="s">
@@ -33896,7 +33977,7 @@
       <c r="L190" s="3">
         <v>313</v>
       </c>
-      <c r="M190" s="1">
+      <c r="M190" s="58">
         <v>560</v>
       </c>
       <c r="N190" s="1" t="s">
@@ -33940,7 +34021,7 @@
       <c r="L191" s="3">
         <v>313</v>
       </c>
-      <c r="M191" s="1">
+      <c r="M191" s="58">
         <v>570</v>
       </c>
       <c r="N191" s="1" t="s">
@@ -33984,7 +34065,7 @@
       <c r="L192" s="3">
         <v>313</v>
       </c>
-      <c r="M192" s="1">
+      <c r="M192" s="58">
         <v>580</v>
       </c>
       <c r="N192" s="1" t="s">
@@ -34015,6 +34096,7 @@
       </c>
       <c r="K193" s="2"/>
       <c r="L193" s="3"/>
+      <c r="M193" s="58"/>
     </row>
     <row r="194" spans="1:14" ht="13.5" customHeight="1">
       <c r="A194" s="1" t="s">
@@ -34040,6 +34122,7 @@
       </c>
       <c r="K194" s="2"/>
       <c r="L194" s="3"/>
+      <c r="M194" s="58"/>
     </row>
     <row r="195" spans="1:14" ht="13.5" customHeight="1">
       <c r="A195" s="1" t="s">
@@ -34078,7 +34161,7 @@
       <c r="L195" s="3">
         <v>311</v>
       </c>
-      <c r="M195" s="1">
+      <c r="M195" s="58">
         <v>611</v>
       </c>
       <c r="N195" s="1" t="s">
@@ -34122,7 +34205,7 @@
       <c r="L196" s="3">
         <v>311</v>
       </c>
-      <c r="M196" s="1">
+      <c r="M196" s="58">
         <v>615</v>
       </c>
       <c r="N196" s="1" t="s">
@@ -34153,6 +34236,7 @@
       </c>
       <c r="K197" s="2"/>
       <c r="L197" s="3"/>
+      <c r="M197" s="58"/>
     </row>
     <row r="198" spans="1:14" ht="13.5" customHeight="1">
       <c r="A198" s="1" t="s">
@@ -34191,7 +34275,7 @@
       <c r="L198" s="3">
         <v>312</v>
       </c>
-      <c r="M198" s="1">
+      <c r="M198" s="58">
         <v>621</v>
       </c>
       <c r="N198" s="1" t="s">
@@ -34235,7 +34319,7 @@
       <c r="L199" s="3">
         <v>312</v>
       </c>
-      <c r="M199" s="1">
+      <c r="M199" s="58">
         <v>625</v>
       </c>
       <c r="N199" s="1" t="s">
@@ -34279,7 +34363,7 @@
       <c r="L200" s="3">
         <v>311</v>
       </c>
-      <c r="M200" s="1">
+      <c r="M200" s="58">
         <v>630</v>
       </c>
       <c r="N200" s="1" t="s">
@@ -34323,7 +34407,7 @@
       <c r="L201" s="3">
         <v>311</v>
       </c>
-      <c r="M201" s="1">
+      <c r="M201" s="58">
         <v>640</v>
       </c>
       <c r="N201" s="1" t="s">
@@ -34367,7 +34451,7 @@
       <c r="L202" s="3">
         <v>313</v>
       </c>
-      <c r="M202" s="1">
+      <c r="M202" s="58">
         <v>650</v>
       </c>
       <c r="N202" s="1" t="s">
@@ -34411,7 +34495,7 @@
       <c r="L203" s="3">
         <v>313</v>
       </c>
-      <c r="M203" s="1">
+      <c r="M203" s="58">
         <v>660</v>
       </c>
       <c r="N203" s="1" t="s">
@@ -34455,7 +34539,7 @@
       <c r="L204" s="3">
         <v>313</v>
       </c>
-      <c r="M204" s="1">
+      <c r="M204" s="58">
         <v>670</v>
       </c>
       <c r="N204" s="1" t="s">
@@ -34499,7 +34583,7 @@
       <c r="L205" s="3">
         <v>313</v>
       </c>
-      <c r="M205" s="1">
+      <c r="M205" s="58">
         <v>680</v>
       </c>
       <c r="N205" s="1" t="s">
@@ -34530,6 +34614,7 @@
       </c>
       <c r="K206" s="2"/>
       <c r="L206" s="3"/>
+      <c r="M206" s="58"/>
     </row>
     <row r="207" spans="1:14" ht="13.5" customHeight="1">
       <c r="A207" s="1" t="s">
@@ -34555,6 +34640,7 @@
       </c>
       <c r="K207" s="2"/>
       <c r="L207" s="3"/>
+      <c r="M207" s="58"/>
     </row>
     <row r="208" spans="1:14" ht="13.5" customHeight="1">
       <c r="A208" s="1" t="s">
@@ -34593,7 +34679,7 @@
       <c r="L208" s="3">
         <v>311</v>
       </c>
-      <c r="M208" s="1">
+      <c r="M208" s="58">
         <v>711</v>
       </c>
       <c r="N208" s="1" t="s">
@@ -34637,7 +34723,7 @@
       <c r="L209" s="3">
         <v>324</v>
       </c>
-      <c r="M209" s="1">
+      <c r="M209" s="58">
         <v>715</v>
       </c>
       <c r="N209" s="1" t="s">
@@ -34668,6 +34754,7 @@
       </c>
       <c r="K210" s="2"/>
       <c r="L210" s="3"/>
+      <c r="M210" s="58"/>
     </row>
     <row r="211" spans="1:14" ht="13.5" customHeight="1">
       <c r="A211" s="1" t="s">
@@ -34706,7 +34793,7 @@
       <c r="L211" s="3">
         <v>312</v>
       </c>
-      <c r="M211" s="1">
+      <c r="M211" s="58">
         <v>721</v>
       </c>
       <c r="N211" s="1" t="s">
@@ -34750,7 +34837,7 @@
       <c r="L212" s="3">
         <v>324</v>
       </c>
-      <c r="M212" s="1">
+      <c r="M212" s="58">
         <v>725</v>
       </c>
       <c r="N212" s="1" t="s">
@@ -34794,7 +34881,7 @@
       <c r="L213" s="3">
         <v>324</v>
       </c>
-      <c r="M213" s="1">
+      <c r="M213" s="58">
         <v>730</v>
       </c>
       <c r="N213" s="1" t="s">
@@ -34838,7 +34925,7 @@
       <c r="L214" s="3">
         <v>324</v>
       </c>
-      <c r="M214" s="1">
+      <c r="M214" s="58">
         <v>740</v>
       </c>
       <c r="N214" s="1" t="s">
@@ -34882,7 +34969,7 @@
       <c r="L215" s="3">
         <v>324</v>
       </c>
-      <c r="M215" s="1">
+      <c r="M215" s="58">
         <v>750</v>
       </c>
       <c r="N215" s="1" t="s">
@@ -34926,7 +35013,7 @@
       <c r="L216" s="3">
         <v>324</v>
       </c>
-      <c r="M216" s="1">
+      <c r="M216" s="58">
         <v>760</v>
       </c>
       <c r="N216" s="1" t="s">
@@ -34970,7 +35057,7 @@
       <c r="L217" s="3">
         <v>324</v>
       </c>
-      <c r="M217" s="1">
+      <c r="M217" s="58">
         <v>770</v>
       </c>
       <c r="N217" s="1" t="s">
@@ -35014,7 +35101,7 @@
       <c r="L218" s="3">
         <v>324</v>
       </c>
-      <c r="M218" s="1">
+      <c r="M218" s="58">
         <v>780</v>
       </c>
       <c r="N218" s="1" t="s">
@@ -35045,6 +35132,7 @@
       </c>
       <c r="K219" s="2"/>
       <c r="L219" s="3"/>
+      <c r="M219" s="58"/>
     </row>
     <row r="220" spans="1:14" ht="13.5" customHeight="1">
       <c r="A220" s="1" t="s">
@@ -35070,6 +35158,7 @@
       </c>
       <c r="K220" s="2"/>
       <c r="L220" s="3"/>
+      <c r="M220" s="58"/>
     </row>
     <row r="221" spans="1:14" ht="13.5" customHeight="1">
       <c r="A221" s="1" t="s">
@@ -35108,7 +35197,7 @@
       <c r="L221" s="3">
         <v>311</v>
       </c>
-      <c r="M221" s="1">
+      <c r="M221" s="58">
         <v>811</v>
       </c>
       <c r="N221" s="1" t="s">
@@ -35152,7 +35241,7 @@
       <c r="L222" s="3">
         <v>244</v>
       </c>
-      <c r="M222" s="1">
+      <c r="M222" s="58">
         <v>815</v>
       </c>
       <c r="N222" s="1" t="s">
@@ -35183,6 +35272,7 @@
       </c>
       <c r="K223" s="2"/>
       <c r="L223" s="3"/>
+      <c r="M223" s="58"/>
     </row>
     <row r="224" spans="1:14" ht="13.5" customHeight="1">
       <c r="A224" s="1" t="s">
@@ -35221,7 +35311,7 @@
       <c r="L224" s="3">
         <v>312</v>
       </c>
-      <c r="M224" s="1">
+      <c r="M224" s="58">
         <v>821</v>
       </c>
       <c r="N224" s="1" t="s">
@@ -35265,7 +35355,7 @@
       <c r="L225" s="3">
         <v>324</v>
       </c>
-      <c r="M225" s="1">
+      <c r="M225" s="58">
         <v>825</v>
       </c>
       <c r="N225" s="1" t="s">
@@ -35309,7 +35399,7 @@
       <c r="L226" s="3">
         <v>324</v>
       </c>
-      <c r="M226" s="1">
+      <c r="M226" s="58">
         <v>830</v>
       </c>
       <c r="N226" s="1" t="s">
@@ -35353,7 +35443,7 @@
       <c r="L227" s="3">
         <v>324</v>
       </c>
-      <c r="M227" s="1">
+      <c r="M227" s="58">
         <v>840</v>
       </c>
       <c r="N227" s="1" t="s">
@@ -35397,7 +35487,7 @@
       <c r="L228" s="3">
         <v>324</v>
       </c>
-      <c r="M228" s="1">
+      <c r="M228" s="58">
         <v>850</v>
       </c>
       <c r="N228" s="1" t="s">
@@ -35441,7 +35531,7 @@
       <c r="L229" s="3">
         <v>324</v>
       </c>
-      <c r="M229" s="1">
+      <c r="M229" s="58">
         <v>860</v>
       </c>
       <c r="N229" s="1" t="s">
@@ -35485,7 +35575,7 @@
       <c r="L230" s="3">
         <v>324</v>
       </c>
-      <c r="M230" s="1">
+      <c r="M230" s="58">
         <v>870</v>
       </c>
       <c r="N230" s="1" t="s">
@@ -35529,7 +35619,7 @@
       <c r="L231" s="3">
         <v>324</v>
       </c>
-      <c r="M231" s="1">
+      <c r="M231" s="58">
         <v>880</v>
       </c>
       <c r="N231" s="1" t="s">
@@ -35560,6 +35650,7 @@
       </c>
       <c r="K232" s="2"/>
       <c r="L232" s="3"/>
+      <c r="M232" s="58"/>
     </row>
     <row r="233" spans="1:14" ht="13.5" customHeight="1">
       <c r="A233" s="1" t="s">
@@ -35598,7 +35689,7 @@
       <c r="L233" s="3">
         <v>244</v>
       </c>
-      <c r="M233" s="1">
+      <c r="M233" s="58">
         <v>891</v>
       </c>
       <c r="N233" s="1" t="s">
@@ -35642,7 +35733,7 @@
       <c r="L234" s="3">
         <v>244</v>
       </c>
-      <c r="M234" s="1">
+      <c r="M234" s="58">
         <v>895</v>
       </c>
       <c r="N234" s="1" t="s">
@@ -35686,6 +35777,7 @@
       <c r="L235" s="3">
         <v>324</v>
       </c>
+      <c r="M235" s="58"/>
     </row>
     <row r="236" spans="1:14" ht="13.5" customHeight="1">
       <c r="A236" s="1" t="s">
@@ -35711,6 +35803,7 @@
       </c>
       <c r="K236" s="2"/>
       <c r="L236" s="3"/>
+      <c r="M236" s="58"/>
     </row>
     <row r="237" spans="1:14" ht="13.5" customHeight="1">
       <c r="A237" s="1" t="s">
@@ -35749,7 +35842,7 @@
       <c r="L237" s="3">
         <v>323</v>
       </c>
-      <c r="M237" s="1">
+      <c r="M237" s="58">
         <v>911</v>
       </c>
       <c r="N237" s="1" t="s">
@@ -35780,6 +35873,7 @@
       </c>
       <c r="K238" s="2"/>
       <c r="L238" s="3"/>
+      <c r="M238" s="58"/>
     </row>
     <row r="239" spans="1:14" ht="13.5" customHeight="1">
       <c r="A239" s="1" t="s">
@@ -35818,7 +35912,7 @@
       <c r="L239" s="3">
         <v>323</v>
       </c>
-      <c r="M239" s="1">
+      <c r="M239" s="58">
         <v>915</v>
       </c>
       <c r="N239" s="1" t="s">
@@ -35862,7 +35956,7 @@
       <c r="L240" s="3">
         <v>333</v>
       </c>
-      <c r="M240" s="1">
+      <c r="M240" s="58">
         <v>917</v>
       </c>
       <c r="N240" s="1" t="s">
@@ -35893,6 +35987,7 @@
       </c>
       <c r="K241" s="2"/>
       <c r="L241" s="3"/>
+      <c r="M241" s="58"/>
     </row>
     <row r="242" spans="1:14" ht="13.5" customHeight="1">
       <c r="A242" s="1" t="s">
@@ -35931,7 +36026,7 @@
       <c r="L242" s="3">
         <v>321</v>
       </c>
-      <c r="M242" s="1">
+      <c r="M242" s="58">
         <v>921</v>
       </c>
       <c r="N242" s="1" t="s">
@@ -35975,7 +36070,7 @@
       <c r="L243" s="3">
         <v>333</v>
       </c>
-      <c r="M243" s="1">
+      <c r="M243" s="58">
         <v>925</v>
       </c>
       <c r="N243" s="1" t="s">
@@ -36006,7 +36101,7 @@
       </c>
       <c r="K244" s="2"/>
       <c r="L244" s="3"/>
-      <c r="M244" s="1">
+      <c r="M244" s="58">
         <v>950</v>
       </c>
       <c r="N244" s="1" t="s">
@@ -36050,7 +36145,7 @@
       <c r="L245" s="3">
         <v>331</v>
       </c>
-      <c r="M245" s="1">
+      <c r="M245" s="58">
         <v>931</v>
       </c>
       <c r="N245" s="1" t="s">
@@ -36094,7 +36189,7 @@
       <c r="L246" s="3">
         <v>332</v>
       </c>
-      <c r="M246" s="1">
+      <c r="M246" s="58">
         <v>941</v>
       </c>
       <c r="N246" s="1" t="s">
@@ -36138,7 +36233,7 @@
       <c r="L247" s="3">
         <v>332</v>
       </c>
-      <c r="M247" s="1">
+      <c r="M247" s="58">
         <v>945</v>
       </c>
       <c r="N247" s="1" t="s">
@@ -36182,7 +36277,7 @@
       <c r="L248" s="3">
         <v>333</v>
       </c>
-      <c r="M248" s="1">
+      <c r="M248" s="58">
         <v>933</v>
       </c>
       <c r="N248" s="1" t="s">
@@ -36226,7 +36321,7 @@
       <c r="L249" s="3">
         <v>334</v>
       </c>
-      <c r="M249" s="1">
+      <c r="M249" s="58">
         <v>934</v>
       </c>
       <c r="N249" s="1" t="s">
@@ -36270,7 +36365,7 @@
       <c r="L250" s="3">
         <v>333</v>
       </c>
-      <c r="M250" s="1">
+      <c r="M250" s="58">
         <v>1007</v>
       </c>
       <c r="N250" s="1" t="s">
@@ -36314,7 +36409,7 @@
       <c r="L251" s="3">
         <v>333</v>
       </c>
-      <c r="M251" s="1">
+      <c r="M251" s="58">
         <v>1006</v>
       </c>
       <c r="N251" s="1" t="s">
@@ -36358,7 +36453,7 @@
       <c r="L252" s="3">
         <v>333</v>
       </c>
-      <c r="M252" s="1">
+      <c r="M252" s="58">
         <v>935</v>
       </c>
       <c r="N252" s="1" t="s">
@@ -39359,6 +39454,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup scale="0" orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>